<commit_message>
Update raw data to increase variability in group size
</commit_message>
<xml_diff>
--- a/data-raw/data-raw.xlsx
+++ b/data-raw/data-raw.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolehill/Code/bisonpictools/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E484740-6C5C-864C-8062-15D350DBACC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1E3C1DF-1257-8A4D-AB37-DB41247FA063}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="500" windowWidth="25320" windowHeight="13920" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -534,7 +534,7 @@
   <dimension ref="A1:T13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="91" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="T14" sqref="T14"/>
+      <selection activeCell="T10" sqref="T10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -752,31 +752,31 @@
         <v>1</v>
       </c>
       <c r="H4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J4">
         <v>0</v>
       </c>
       <c r="K4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O4">
         <v>1</v>
       </c>
       <c r="P4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q4">
         <v>0</v>
@@ -1124,28 +1124,28 @@
         <v>1</v>
       </c>
       <c r="H10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I10">
         <v>1</v>
       </c>
       <c r="J10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K10">
         <v>0</v>
       </c>
       <c r="L10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N10">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="O10">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P10">
         <v>0</v>

</xml_diff>